<commit_message>
add Table numbers to SI tables
</commit_message>
<xml_diff>
--- a/data/geochron/ECMB_apatite.xlsx
+++ b/data/geochron/ECMB_apatite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Laurentia/0000_Github/2021_ECMB/data/geochron/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B120F7-F9F6-4D48-9C48-9FA647076F86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E614DA8-6CAE-AF43-864A-591ABB241051}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="37680" windowHeight="26900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -695,7 +695,7 @@
     <t>Strikethrough indicates data discarded because final integrations were not flat</t>
   </si>
   <si>
-    <t>U-Pb apatite data</t>
+    <t>Table S2: Apatite U-Pb data</t>
   </si>
 </sst>
 </file>
@@ -1457,7 +1457,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T38" sqref="T38"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>

</xml_diff>